<commit_message>
fixed the bug when decoding gbk and utf-8; add README
</commit_message>
<xml_diff>
--- a/database/wchoiceQ.xlsx
+++ b/database/wchoiceQ.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -640,6 +640,119 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>The result of “ab”+”c”*2 is ()</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>abc2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>abcabc</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>abcc</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ababcc</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Which of the following options is not correct about the following code  ()
+fname = input("请输入要写入的文件: ")
+fo = open(fname, "w+")
+ls = ["清明时节雨纷纷，","路上行人欲断魂，","借问酒家何处有？","牧童遥指杏花村。"]
+fo.writelines(ls)
+fo.seek(0)
+for line in fo:
+    print(line)
+fo.close()</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>fo. seek (0) can be omitted，the output is unchanged.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>fo. writelines (ls) writes the ls list whose elements are all strings to a file</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>The main function of the code is to write a list type to the file and print out the result</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>When executing the code, enter "Qingming.txt" from the keyboard, and Qingming.txt is created</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>关于Python程序中与“缩进”有关的说法中，以下选项中正确的是</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>缩进统一为4个空格</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>缩进可以用在任何语句之后，表示语句间的包含关系</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>缩进在程序中长度统一且强制使用</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>缩进是非强制性的，仅为了提高代码可读性</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>